<commit_message>
Tu mensaje de commit
</commit_message>
<xml_diff>
--- a/Base/consolidado.xlsx
+++ b/Base/consolidado.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5569,6 +5569,342 @@
         </is>
       </c>
       <c r="J107" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Arthur Hassuma</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>9</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>314457</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Arthur Hassuma</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>9</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>315282</v>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Arthur Hassuma</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>9</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>315511</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Arthur Hassuma</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>9</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>315663</v>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Higor Cruz</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>9</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>315374</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Luan Pierry</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>9</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>315638</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Luan Pierry</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>9</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>315817</v>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
         <is>
           <t>Willian Jones</t>
         </is>
@@ -5585,7 +5921,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:J158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11492,7 +11828,7 @@
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>Resolvido</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -11780,7 +12116,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>Resolvido</t>
         </is>
       </c>
       <c r="J129" t="inlineStr">
@@ -12024,6 +12360,1158 @@
         </is>
       </c>
       <c r="J134" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Erick Silva</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>9</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>315595</v>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Erick Silva</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>9</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>315683</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Erick Silva</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>9</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>315754</v>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Gustavo Linpiski</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>9</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>315377</v>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Gustavo Linpiski</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>9</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>315966</v>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Jorgenaldo Reis</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>9</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>315952</v>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Jorgenaldo Reis</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>9</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>316151</v>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Jorgenaldo Reis</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>9</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>315807</v>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Jorgenaldo Reis</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>9</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>316110</v>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>Resolvido</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Jose Acevedo</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>9</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>06/12/2024</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>315183</v>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Alana Neris</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>10</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>316702</v>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>12/2024</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Alana Neris</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>10</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
+        <v>316765</v>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>12/2024</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Alana Neris</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>10</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
+        <v>316993</v>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>12/2024</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Edson Campos</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>10</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>315916</v>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Edson Campos</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>10</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>315812</v>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Erick Silva</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>10</v>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>316732</v>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>12/2024</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Erick Silva</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>10</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F151" t="n">
+        <v>316626</v>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>12/2024</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Erick Silva</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>10</v>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>316501</v>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>12/2024</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Gabriel Lopez</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>10</v>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>316114</v>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Jacyr Popenda</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>10</v>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>316940</v>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>12/2024</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Jorgenaldo Reis</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>10</v>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F155" t="n">
+        <v>315817</v>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Jose Acevedo</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>10</v>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>316763</v>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>12/2024</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Lourival Moizés</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>10</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F157" t="n">
+        <v>315310</v>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Lourival Moizés</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>10</v>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>13/12/2024</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>315758</v>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>11/2024</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
         <is>
           <t>Emerson Simette</t>
         </is>

</xml_diff>

<commit_message>
Mensagem explicando o que foi feito
</commit_message>
<xml_diff>
--- a/Base/consolidado.xlsx
+++ b/Base/consolidado.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1200,6 +1200,465 @@
         </is>
       </c>
       <c r="K15" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Higor Cruz</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>322731</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Higor Cruz</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>322526</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Higor Cruz</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D18" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>321751</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Higor Cruz</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D19" t="n">
+        <v>5</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>321760</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Arthur Hassuma</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D20" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>322877</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Luan Pierry</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D21" t="n">
+        <v>5</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>322586</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Luan Pierry</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D22" t="n">
+        <v>5</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>322053</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Mara Neves</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>322696</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Willian Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>SPN</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Mara Neves</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D24" t="n">
+        <v>5</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>322164</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>Willian Jones</t>
         </is>
@@ -1216,7 +1675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3168,6 +3627,567 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Lourival Moizés</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D39" t="n">
+        <v>5</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>322346</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Guilherme Worel</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D40" t="n">
+        <v>5</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>321835</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Guilherme Worel</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D41" t="n">
+        <v>5</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>322897</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Guilherme Worel</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D42" t="n">
+        <v>5</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>322991</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Jorgenaldo Reis</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D43" t="n">
+        <v>5</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>322655</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Jose Acevedo</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D44" t="n">
+        <v>5</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>322167</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Erick da Silva</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D45" t="n">
+        <v>5</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>322927</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Erick da Silva</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D46" t="n">
+        <v>5</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>322759</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Erick da Silva</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D47" t="n">
+        <v>5</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>322764</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Erick da Silva</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D48" t="n">
+        <v>5</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>322804</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ITI</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Lourival Moizés</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D49" t="n">
+        <v>5</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>321811</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>01/2025</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Emerson Simette</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>